<commit_message>
Clean up commit for device switching
</commit_message>
<xml_diff>
--- a/device-switching/experiments/production/baseline/stimuli.xlsx
+++ b/device-switching/experiments/production/baseline/stimuli.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dbrau\Dropbox (Lehigh University)\post_doc\professional\NHI\nhi-experiments\device-switching\experiments\production\baseline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9E60036E-4951-4F6E-92CD-EC890F5D3724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6AA8B2B-7EDF-4D91-A3C9-40228CC2E866}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,16 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="8">
-  <si>
-    <t>stimulus</t>
-  </si>
-  <si>
-    <t>display</t>
-  </si>
-  <si>
-    <t>cor_mag_resp</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="16">
   <si>
     <t>j</t>
   </si>
@@ -45,10 +36,43 @@
     <t>cor_par_resp</t>
   </si>
   <si>
-    <t>d</t>
-  </si>
-  <si>
     <t>f</t>
+  </si>
+  <si>
+    <t>number_stimulus</t>
+  </si>
+  <si>
+    <t>letter_stimulus</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>U</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>cor_number_resp</t>
+  </si>
+  <si>
+    <t>g</t>
   </si>
 </sst>
 </file>
@@ -369,251 +393,252 @@
   <dimension ref="A1:D17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>1</v>
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
       </c>
       <c r="C4" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
-      </c>
-      <c r="B5">
-        <v>1</v>
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>6</v>
       </c>
-      <c r="B6">
-        <v>1</v>
+      <c r="B6" t="s">
+        <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>7</v>
       </c>
-      <c r="B7">
-        <v>1</v>
+      <c r="B7" t="s">
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>8</v>
       </c>
-      <c r="B8">
-        <v>1</v>
+      <c r="B8" t="s">
+        <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>9</v>
       </c>
-      <c r="B9">
-        <v>1</v>
+      <c r="B9" t="s">
+        <v>13</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>1</v>
-      </c>
-      <c r="B10">
-        <v>0</v>
+        <v>2</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2</v>
-      </c>
-      <c r="B11">
-        <v>0</v>
+        <v>3</v>
+      </c>
+      <c r="B11" t="s">
+        <v>7</v>
       </c>
       <c r="C11" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>3</v>
-      </c>
-      <c r="B12">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="B12" t="s">
+        <v>8</v>
       </c>
       <c r="C12" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>4</v>
-      </c>
-      <c r="B13">
-        <v>0</v>
+        <v>5</v>
+      </c>
+      <c r="B13" t="s">
+        <v>9</v>
       </c>
       <c r="C13" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>6</v>
       </c>
-      <c r="B14">
-        <v>0</v>
+      <c r="B14" t="s">
+        <v>10</v>
       </c>
       <c r="C14" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D14" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>7</v>
       </c>
-      <c r="B15">
-        <v>0</v>
+      <c r="B15" t="s">
+        <v>11</v>
       </c>
       <c r="C15" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>8</v>
       </c>
-      <c r="B16">
-        <v>0</v>
+      <c r="B16" t="s">
+        <v>12</v>
       </c>
       <c r="C16" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D16" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>9</v>
       </c>
-      <c r="B17">
-        <v>0</v>
+      <c r="B17" t="s">
+        <v>13</v>
       </c>
       <c r="C17" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>7</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>